<commit_message>
hopefully some original work in here
</commit_message>
<xml_diff>
--- a/work/CTet/DailyMail.xlsx
+++ b/work/CTet/DailyMail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="6880" yWindow="-80" windowWidth="21600" windowHeight="13680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,248 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="91">
+  <si>
+    <t xml:space="preserve">household poisons listed inc bleach weedkiller, polish, disinfectant creosote paraffin, asprins. Ctet and turpentine described as attacking the lungs. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Make your own laboratory with jam jar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fri</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Albright &amp; Wilson, leading chem mfcr in the country, emply 5000+ in 7 production plants, products include phsophorus, phosphoric acid and phospates, c4tet, sulphuric acid. Interesting as  Marchon chem products also in same strip - article on that page is profile of colgate palmolive and director EH Little</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Albright &amp; Wilson no fire risk, princiapl solvents used by dry cleaners engineers and rubber mfcrs, also fire exting. One of many industrial chems made by A&amp;W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Don't cry over spilt ink</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Now to get rid of the stains</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>in context of being saved by a gallant naval officer sprinkling salt on writers dress. Mentions oxalic acid, c4Tet, borax, ammonia, bleach, proprietary brands (though unnamed)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Is your home a child-killer? A DM investigation … and wardning. side column in article about dangerous houshold products, lists sodium hypochlorite, oven cleaner, stain remover. Mentions inadequate warning labels</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Call for curb on danger chemical</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scientists underestimated danger of 111 trichloroethane, highligted by DM/FOE investigation. Chris Patten env sec, wants t and ctet to be restricted worldwide w CFCs. UN pressing for ban by 2000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">page of cinema, ads for wine, jelly, lemonade, crossword "Specially for women. Stain removal in the context of having a house full of evacuees. C4Tet in context of egg on no-washable material. Gum, apply white of egg. Ink on dress fabrics tablecloth, tomato juice rubbed in sprinkle with salt and steam. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>05.11.58</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15.06.90</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>These could kill you</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>24.06.71</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">fashion page - in refrence to hairpiece - expert advice from owner of 10 salons, save time and money, dunk it in and out of a bowl of ctet from most chems, near open window, stuff smells stong. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">fashion page - in reference to hairpiece - clean monthly by dunking in ctet near open window as the fumes can be dangerous. Never smoke or work near naked flame. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ctet as solvent for silicone, waterproofing fishing flies. Assume proprietary waterproofers? Jam jar is for testing flies in water. Page has ents listings, comic strips </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fascination for smell, had cleaned tracks of trainset, went to bed clutching rag to his face.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Your top-knot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.03.64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Four heads on one girl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>05.12.64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Asprins are the biggest killer of under 5's</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>25.04.66</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>anaesthetic, never to a woman in stays, hairdressing poistion head back is bad, , c4t application causes a sensation of cold to the area it touches, possibly enough to shock the status lympaticus faint / cardiac failure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>03.09.09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Friday</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas War on Vermin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thurs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>02.04.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>31.03.67</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Never let a stain put you on the spot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21.07.54</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boy took poison</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>04.12.54</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">orphan boy drank C4Tet after being badly beaten up, spine fractured. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>29.12.55</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">party time, spills spoil fun. Hydrogen peroxide, c4tet, lighterfuel, prop brand, </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14.11.57</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Foamite, complete protection for chem and oil plants, full range of fire extinguishers inc c4tet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">muddled drug addict possibly drunk ctet by mistake. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>advertising</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Titled char was a drug addict</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Friday</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20.03.59</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Smell kills boy aged 6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20.10.62</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multiple display ads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>26.10.44</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Nuswift  fire extinguishers, contains no acid, operated by CO2 (Water), C4Tet extinguishers also available. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prize flowers poisoned</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>03.11.47</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sabotage, betting on flower show, jealous fellow exhibitor, expert gardener knowledge f chemicals. C4Tet is one of the few commonly used substances that would give off fumes destructive to chrysanths. Used widely in silk dye works, industry in Macclesfield. sab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multiple display ads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.12.47</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>27.03.1950</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">UV light will show up halo round spots, so don't lie to dry cleaners. Suthetic materials, r. </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -146,238 +382,6 @@
   </si>
   <si>
     <t>Fatal Shampoo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>anaesthetic, never to a woman in stays, hairdressing poistion head back is bad, , c4t application causes a sensation of cold to the area it touches, possibly enough to shock the status lympaticus faint / cardiac failure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>03.09.09</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Friday</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas War on Vermin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Thurs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>02.04.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>31.03.67</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Never let a stain put you on the spot</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>21.07.54</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Boy took poison</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>04.12.54</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">orphan boy drank C4Tet after being badly beaten up, spine fractured. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Now to get rid of the stains</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>29.12.55</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">party time, spills spoil fun. Hydrogen peroxide, c4tet, lighterfuel, prop brand, </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>14.11.57</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Foamite, complete protection for chem and oil plants, full range of fire extinguishers inc c4tet</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">muddled drug addict possibly drunk ctet by mistake. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>advertising</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Titled char was a drug addict</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Friday</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20.03.59</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Smell kills boy aged 6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20.10.62</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Multiple display ads</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>26.10.44</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Nuswift  fire extinguishers, contains no acid, operated by CO2 (Water), C4Tet extinguishers also available. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prize flowers poisoned</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>03.11.47</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sabotage, betting on flower show, jealous fellow exhibitor, expert gardener knowledge f chemicals. C4Tet is one of the few commonly used substances that would give off fumes destructive to chrysanths. Used widely in silk dye works, industry in Macclesfield. sab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Multiple display ads</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>19.12.47</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Albright &amp; Wilson no fire risk, princiapl sovents used by dry cleaners engineers and rubber mfcrs, also fire exting. One of many industrial chems made by A&amp;W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>27.03.1950</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>in context of being saved by a gallant naval officer sprinkling salt on writers dress. Mentions oxalic acid, c4Tet, borax, ammonia, bleach, proprietary brands (though unnamed)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Is your home a child-killer? A DM investigation … and wardning. side column in article about dangerous houshold products, lists sodium hypochlorite, oven cleaner, stain remover. Mentions inadequate warning labels</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Call for curb on danger chemical</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>scientists underestimated danger of 111 trichloroethane, highligted by DM/FOE investigation. Chris Patten env sec, wants t and ctet to be restricted worldwide w CFCs. UN pressing for ban by 2000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">page of cinema, ads for wine, jelly, lemonade, crossword "Specially for women. Stain removal in the context of having a house full of evacuees. C4Tet in context of egg on no-washable material. Gum, apply white of egg. Ink on dress fabrics tablecloth, tomato juice rubbed in sprinkle with salt and steam. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>05.11.58</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>15.06.90</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>These could kill you</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>24.06.71</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">fashion page - in refrence to hairpiece - expert advice from owner of 10 salons, save time and money, dunk it in and out of a bowl of ctet from most chems, near open window, stuff smells stong. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">fashion page - in reference to hairpiece - clean monthly by dunking in ctet near open window as the fumes can be dangerous. Never smoke or work near naked flame. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ctet as solvent for silicone, waterproofing fishing flies. Assume proprietary waterproofers? Jam jar is for testing flies in water. Page has ents listings, comic strips </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fascination for smell, had cleaned tracks of trainset, went to bed clutching rag to his face.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Your top-knot</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>19.03.64</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Four heads on one girl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>05.12.64</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Asprins are the biggest killer of under 5's</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>25.04.66</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">household poisons listed inc bleach weedkiller, polish, disinfectant creosote paraffin, asprins. Ctet and turpentine described as attacking the lungs. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Make your own laboratory with jam jar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fri</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -750,494 +754,498 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="F6" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" t="s">
         <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
         <v>65</v>
       </c>
-      <c r="E12" t="s">
-        <v>6</v>
-      </c>
       <c r="F12" t="s">
-        <v>66</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B13">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="F14" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="F15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="B16">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B17">
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="F17" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B18">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B19">
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="F19" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B20">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="F21" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="F22" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="D23" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="F23" t="s">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="B24">
         <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="F24" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="B25">
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="F25" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B26">
         <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="F26" t="s">
-        <v>71</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>